<commit_message>
Deleted "_dict" from all capital variable names.
</commit_message>
<xml_diff>
--- a/inputs/scenario_test1.xlsx
+++ b/inputs/scenario_test1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
@@ -731,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding features for tenure
</commit_message>
<xml_diff>
--- a/inputs/scenario_test1.xlsx
+++ b/inputs/scenario_test1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Tenure Pref</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>Tenure</t>
   </si>
 </sst>
 </file>
@@ -509,15 +521,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +570,14 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -598,8 +617,14 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -622,7 +647,7 @@
         <v>100000</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -639,8 +664,14 @@
       <c r="M3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -680,8 +711,14 @@
       <c r="M4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -720,6 +757,12 @@
       </c>
       <c r="M5" t="s">
         <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +775,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A Household()'s Residence() now gets put into a housing stock FilterStore at initiation
* Modified Household() class (entities.py) so that
    * Residence() is set within in a method, rather than directly in
the __init__ method
    * After household’s reisdence is set, that residence is placed into
a SimPy FilterStore that acts as an occupied housing stock
    * In this way both the household and the occupied housing stock has
the same pointer in memory of the corresponding Residence() object
</commit_message>
<xml_diff>
--- a/inputs/scenario_test1.xlsx
+++ b/inputs/scenario_test1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Tenure Pref</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Own</t>
+  </si>
+  <si>
+    <t>Tenure</t>
   </si>
 </sst>
 </file>
@@ -509,15 +521,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +570,14 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -598,8 +617,14 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -622,7 +647,7 @@
         <v>100000</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>5</v>
@@ -639,8 +664,14 @@
       <c r="M3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -680,8 +711,14 @@
       <c r="M4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -720,6 +757,12 @@
       </c>
       <c r="M5" t="s">
         <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +775,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>